<commit_message>
Code for publication. Updated with multiple analysis approaches.
</commit_message>
<xml_diff>
--- a/2103 - data - cards.xlsx
+++ b/2103 - data - cards.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu.sharepoint.com/teams/nottingham.lab/Shared Documents/Data/DL/2021/2103 - Reflective mulch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu.sharepoint.com/teams/nottingham.lab/Shared Documents/Publications/In progress/2003 - 2103 Reflective implementation/reproduciblecode/2003_reflectivepear/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="11024" documentId="6_{B355563A-835F-4215-ADB0-038B950DB297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81CAB382-E5B9-454B-A56C-CF88667BEFC2}"/>
@@ -7985,7 +7985,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
@@ -37446,9 +37446,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37675,19 +37678,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB559EE5-4696-488D-B853-F9EDC9FBCCA0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B44D486-D049-45E2-B9C4-2EAF4218C713}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37712,9 +37711,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B44D486-D049-45E2-B9C4-2EAF4218C713}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB559EE5-4696-488D-B853-F9EDC9FBCCA0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>